<commit_message>
Updated Notes & Burndown Sprint 3
</commit_message>
<xml_diff>
--- a/Project Documentation/Burn_Down-Sprint-3.xlsx
+++ b/Project Documentation/Burn_Down-Sprint-3.xlsx
@@ -214,19 +214,19 @@
                   <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>51.666666666666664</c:v>
+                  <c:v>49.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41.333333333333329</c:v>
+                  <c:v>37.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.999999999999993</c:v>
+                  <c:v>24.800000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.666666666666657</c:v>
+                  <c:v>12.400000000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.333333333333323</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -307,7 +307,7 @@
                   <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1507,7 +1507,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1531,8 +1531,8 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <f>B1-62/6</f>
-        <v>51.666666666666664</v>
+        <f>B1-62/5</f>
+        <v>49.6</v>
       </c>
       <c r="C2">
         <v>42</v>
@@ -1543,11 +1543,11 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <f>B2-62/6</f>
-        <v>41.333333333333329</v>
+        <f>B2-62/5</f>
+        <v>37.200000000000003</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1555,8 +1555,8 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <f>B3-62/6</f>
-        <v>30.999999999999993</v>
+        <f>B3-62/5</f>
+        <v>24.800000000000004</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1567,8 +1567,8 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <f>B4-62/6</f>
-        <v>20.666666666666657</v>
+        <f>B4-62/5</f>
+        <v>12.400000000000004</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1579,8 +1579,8 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <f>B5-62/6</f>
-        <v>10.333333333333323</v>
+        <f>B5-62/5</f>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>0</v>

</xml_diff>

<commit_message>
Updated Burnchart & Notes3
</commit_message>
<xml_diff>
--- a/Project Documentation/Burn_Down-Sprint-3.xlsx
+++ b/Project Documentation/Burn_Down-Sprint-3.xlsx
@@ -168,14 +168,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Munka1!$A$1:$A$7</c15:sqref>
+                    <c15:sqref>Munka1!$A$1:$A$6</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Munka1!$A$1:$A$6</c:f>
+              <c:f>Munka1!$A$1:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -190,9 +190,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -202,30 +199,27 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Munka1!$B$1:$B$7</c15:sqref>
+                    <c15:sqref>Munka1!$B$1:$B$6</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Munka1!$B$1:$B$6</c:f>
+              <c:f>Munka1!$B$1:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>49.6</c:v>
+                  <c:v>46.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>37.200000000000003</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24.800000000000004</c:v>
+                  <c:v>15.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.400000000000004</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -258,14 +252,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Munka1!$A$1:$A$7</c15:sqref>
+                    <c15:sqref>Munka1!$A$1:$A$6</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Munka1!$A$1:$A$6</c:f>
+              <c:f>Munka1!$A$1:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -280,9 +274,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -292,14 +283,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Munka1!$C$1:$C$7</c15:sqref>
+                    <c15:sqref>Munka1!$C$1:$C$6</c15:sqref>
                   </c15:fullRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Munka1!$C$1:$C$6</c:f>
+              <c:f>Munka1!$C$1:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>62</c:v>
                 </c:pt>
@@ -310,12 +301,9 @@
                   <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -387,6 +375,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.42639457567804023"/>
+              <c:y val="0.86800188860917127"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1177,16 +1173,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>537210</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>62865</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>232410</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>110490</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1504,10 +1500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1531,8 +1527,8 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <f>B1-62/5</f>
-        <v>49.6</v>
+        <f>B1-62/4</f>
+        <v>46.5</v>
       </c>
       <c r="C2">
         <v>42</v>
@@ -1543,8 +1539,8 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <f>B2-62/5</f>
-        <v>37.200000000000003</v>
+        <f>B2-62/4</f>
+        <v>31</v>
       </c>
       <c r="C3">
         <v>32</v>
@@ -1555,11 +1551,11 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <f>B3-62/5</f>
-        <v>24.800000000000004</v>
+        <f>B3-62/4</f>
+        <v>15.5</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1567,22 +1563,10 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <f>B4-62/5</f>
-        <v>12.400000000000004</v>
+        <f>B4-62/4</f>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <f>B5-62/5</f>
-        <v>0</v>
-      </c>
-      <c r="C6">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Burnchart & Notes3-01
</commit_message>
<xml_diff>
--- a/Project Documentation/Burn_Down-Sprint-3.xlsx
+++ b/Project Documentation/Burn_Down-Sprint-3.xlsx
@@ -304,7 +304,7 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1503,7 +1503,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1567,7 +1567,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>